<commit_message>
Incremented Company Name Stop Words
</commit_message>
<xml_diff>
--- a/OperatingDir/results_analysis.xlsx
+++ b/OperatingDir/results_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luislascano01/Documents/Sabadell/Covenants_Matching/AI_VLookUp/OperatingDir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDB1A20-A3D1-B749-A42D-FBBE566733F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DEB9CD-9C78-E047-8C0D-2E3110D74083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="920" windowWidth="17140" windowHeight="21260" xr2:uid="{DB685025-79AF-2A4F-BCE8-327264ED43DA}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{DB685025-79AF-2A4F-BCE8-327264ED43DA}"/>
   </bookViews>
   <sheets>
     <sheet name="results copy" sheetId="1" r:id="rId1"/>
@@ -927,15 +927,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE94CE9-0B09-124F-AA7C-CFB8F7460D71}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -964,22 +961,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>-1</v>
       </c>
       <c r="D2">
-        <v>0.14799999999999999</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="E2">
-        <v>0.125</v>
+        <v>0.375</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f>IF(A2=B2, 1, 0)</f>
@@ -988,22 +985,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>92</v>
+        <v>-1</v>
       </c>
       <c r="D3">
-        <v>0.14799999999999999</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="E3">
-        <v>0.28599999999999998</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f>IF(A3=B3, 1, 0)</f>
@@ -1012,22 +1009,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>28</v>
       </c>
       <c r="D4">
-        <v>0.19400000000000001</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E4">
-        <v>0.42899999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f>IF(A4=B4, 1, 0)</f>
@@ -1036,19 +1033,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="D5">
-        <v>0.221</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="E5">
-        <v>0.375</v>
+        <v>0.222</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1060,19 +1057,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6">
-        <v>0.222</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="E6">
-        <v>0.33300000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1084,22 +1081,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>42</v>
       </c>
       <c r="D7">
-        <v>0.22700000000000001</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="E7">
-        <v>0.28599999999999998</v>
+        <v>0.222</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f>IF(A7=B7, 1, 0)</f>
@@ -1108,22 +1105,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>-1</v>
       </c>
       <c r="D8">
-        <v>0.23599999999999999</v>
+        <v>0.438</v>
       </c>
       <c r="E8">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f>IF(A8=B8, 1, 0)</f>
@@ -1132,16 +1129,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>-1</v>
       </c>
       <c r="D9">
-        <v>0.24299999999999999</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="E9">
         <v>0.42899999999999999</v>
@@ -1156,22 +1153,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>90</v>
+        <v>-1</v>
       </c>
       <c r="D10">
-        <v>0.24399999999999999</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="E10">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f>IF(A10=B10, 1, 0)</f>
@@ -1180,22 +1177,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>-1</v>
+        <v>99</v>
       </c>
       <c r="D11">
-        <v>0.27900000000000003</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="E11">
-        <v>0.375</v>
+        <v>0.125</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
         <f>IF(A11=B11, 1, 0)</f>
@@ -1204,22 +1201,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>-1</v>
       </c>
       <c r="D12">
-        <v>0.28599999999999998</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="E12">
-        <v>0.28599999999999998</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>IF(A12=B12, 1, 0)</f>
@@ -1228,22 +1225,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>-1</v>
+        <v>36</v>
       </c>
       <c r="D13">
-        <v>0.28999999999999998</v>
+        <v>0.879</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0.222</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <f>IF(A13=B13, 1, 0)</f>
@@ -1252,40 +1249,40 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>-1</v>
       </c>
       <c r="D14">
-        <v>0.30499999999999999</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="E14">
-        <v>0.111</v>
+        <v>0.375</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f>IF(A14=B14, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <v>-1</v>
       </c>
       <c r="D15">
-        <v>0.315</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="E15">
         <v>0.25</v>
@@ -1300,22 +1297,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>0.31900000000000001</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="E16">
-        <v>0.25</v>
+        <v>0.222</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <f>IF(A16=B16, 1, 0)</f>
@@ -1348,19 +1345,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>-1</v>
       </c>
       <c r="D18">
-        <v>0.33900000000000002</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="E18">
-        <v>0.375</v>
+        <v>0.222</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1372,19 +1369,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>64</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>0.35399999999999998</v>
+        <v>0.873</v>
       </c>
       <c r="E19">
-        <v>0.42899999999999999</v>
+        <v>0.375</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1396,22 +1393,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>66</v>
+        <v>-1</v>
       </c>
       <c r="D20">
-        <v>0.35699999999999998</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="E20">
-        <v>0.25</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <f>IF(A20=B20, 1, 0)</f>
@@ -1444,22 +1441,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C22">
         <v>-1</v>
       </c>
       <c r="D22">
-        <v>0.371</v>
+        <v>0.222</v>
       </c>
       <c r="E22">
-        <v>0.25</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <f>IF(A22=B22, 1, 0)</f>
@@ -1468,22 +1465,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>24</v>
       </c>
       <c r="D23">
-        <v>0.39700000000000002</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>0.222</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f>IF(A23=B23, 1, 0)</f>
@@ -1492,22 +1489,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D24">
-        <v>0.40200000000000002</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="E24">
-        <v>0.25</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <f>IF(A24=B24, 1, 0)</f>
@@ -1516,19 +1513,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="D25">
-        <v>0.40300000000000002</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="E25">
-        <v>0.125</v>
+        <v>0.222</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1540,19 +1537,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>-1</v>
       </c>
       <c r="D26">
-        <v>0.40500000000000003</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="E26">
-        <v>0.5</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1564,22 +1561,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="C27">
         <v>-1</v>
       </c>
       <c r="D27">
-        <v>0.42599999999999999</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="E27">
-        <v>0.5</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <f>IF(A27=B27, 1, 0)</f>
@@ -1588,19 +1585,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>-1</v>
       </c>
       <c r="D28">
-        <v>0.42699999999999999</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="E28">
-        <v>0.42899999999999999</v>
+        <v>0.375</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1612,22 +1609,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>-1</v>
+        <v>59</v>
       </c>
       <c r="D29">
-        <v>0.438</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="E29">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <f>IF(A29=B29, 1, 0)</f>
@@ -1636,22 +1633,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C30">
         <v>-1</v>
       </c>
       <c r="D30">
-        <v>0.442</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="E30">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <f>IF(A30=B30, 1, 0)</f>
@@ -1660,19 +1657,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="C31">
         <v>-1</v>
       </c>
       <c r="D31">
-        <v>0.443</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="E31">
-        <v>0.2</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1684,19 +1681,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D32">
-        <v>0.44900000000000001</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="E32">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1708,22 +1705,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>-1</v>
       </c>
       <c r="D33">
-        <v>0.45800000000000002</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="E33">
-        <v>0.2</v>
+        <v>0.111</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <f>IF(A33=B33, 1, 0)</f>
@@ -1732,19 +1729,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.46800000000000003</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="E34">
-        <v>0.375</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1756,22 +1753,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="D35">
-        <v>0.49199999999999999</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="E35">
-        <v>0.375</v>
+        <v>0.1</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <f>IF(A35=B35, 1, 0)</f>
@@ -1780,22 +1777,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C36">
         <v>-1</v>
       </c>
       <c r="D36">
-        <v>0.49399999999999999</v>
+        <v>0.371</v>
       </c>
       <c r="E36">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <f>IF(A36=B36, 1, 0)</f>
@@ -1804,19 +1801,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C37">
         <v>-1</v>
       </c>
       <c r="D37">
-        <v>0.52100000000000002</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="E37">
-        <v>0.33300000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1828,22 +1825,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C38">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="D38">
-        <v>0.52500000000000002</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="E38">
         <v>0.222</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
         <f>IF(A38=B38, 1, 0)</f>
@@ -1852,22 +1849,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="C39">
-        <v>-1</v>
+        <v>97</v>
       </c>
       <c r="D39">
-        <v>0.52500000000000002</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="E39">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <f>IF(A39=B39, 1, 0)</f>
@@ -1876,16 +1873,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D40">
-        <v>0.56299999999999994</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="E40">
         <v>0.222</v>
@@ -1900,22 +1897,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>60</v>
+        <v>-1</v>
       </c>
       <c r="D41">
-        <v>0.56499999999999995</v>
+        <v>0.315</v>
       </c>
       <c r="E41">
-        <v>0.222</v>
+        <v>0.25</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <f>IF(A41=B41, 1, 0)</f>
@@ -1924,16 +1921,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C42">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="D42">
-        <v>0.61299999999999999</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="E42">
         <v>0.1</v>
@@ -1948,22 +1945,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C43">
-        <v>59</v>
+        <v>-1</v>
       </c>
       <c r="D43">
-        <v>0.64300000000000002</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="E43">
-        <v>0.25</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
         <f>IF(A43=B43, 1, 0)</f>
@@ -1972,22 +1969,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C44">
-        <v>85</v>
+        <v>-1</v>
       </c>
       <c r="D44">
-        <v>0.65600000000000003</v>
+        <v>0.87</v>
       </c>
       <c r="E44">
-        <v>0.111</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
         <f>IF(A44=B44, 1, 0)</f>
@@ -1996,19 +1993,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C45">
-        <v>88</v>
+        <v>-1</v>
       </c>
       <c r="D45">
-        <v>0.66300000000000003</v>
+        <v>0.442</v>
       </c>
       <c r="E45">
-        <v>0.222</v>
+        <v>0.375</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -2020,19 +2017,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B46">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="D46">
-        <v>0.67800000000000005</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="E46">
-        <v>0.111</v>
+        <v>0.375</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2044,19 +2041,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C47">
         <v>-1</v>
       </c>
       <c r="D47">
-        <v>0.67900000000000005</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="E47">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2068,22 +2065,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C48">
-        <v>73</v>
+        <v>-1</v>
       </c>
       <c r="D48">
-        <v>0.68200000000000005</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="E48">
-        <v>0.111</v>
+        <v>0.2</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <f>IF(A48=B48, 1, 0)</f>
@@ -2092,19 +2089,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="C49">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="D49">
-        <v>0.69099999999999995</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="E49">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2116,19 +2113,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C50">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="D50">
-        <v>0.69599999999999995</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="E50">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -2140,19 +2137,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C51">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="D51">
-        <v>0.7</v>
+        <v>0.221</v>
       </c>
       <c r="E51">
-        <v>0.111</v>
+        <v>0.375</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2164,19 +2161,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="C52">
         <v>-1</v>
       </c>
       <c r="D52">
-        <v>0.73</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="E52">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2188,19 +2185,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C53">
         <v>-1</v>
       </c>
       <c r="D53">
-        <v>0.73299999999999998</v>
+        <v>0.84599999999999997</v>
       </c>
       <c r="E53">
-        <v>0.222</v>
+        <v>0.375</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2212,22 +2209,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C54">
-        <v>-1</v>
+        <v>53</v>
       </c>
       <c r="D54">
-        <v>0.75</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="E54">
-        <v>0.222</v>
+        <v>0.375</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <f>IF(A54=B54, 1, 0)</f>
@@ -2236,19 +2233,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="C55">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="D55">
-        <v>0.753</v>
+        <v>0.7</v>
       </c>
       <c r="E55">
-        <v>0.222</v>
+        <v>0.111</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -2260,22 +2257,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="C56">
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="D56">
-        <v>0.753</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="E56">
-        <v>0.375</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <f>IF(A56=B56, 1, 0)</f>
@@ -2284,46 +2281,46 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C57">
-        <v>97</v>
+        <v>-1</v>
       </c>
       <c r="D57">
-        <v>0.76700000000000002</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="E57">
-        <v>0.1</v>
+        <v>0.111</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
         <f>IF(A57=B57, 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="C58">
-        <v>99</v>
+        <v>-1</v>
       </c>
       <c r="D58">
-        <v>0.77200000000000002</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="E58">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58">
         <f>IF(A58=B58, 1, 0)</f>
@@ -2332,19 +2329,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C59">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D59">
-        <v>0.77800000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="E59">
-        <v>0.222</v>
+        <v>0.25</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2356,19 +2353,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C60">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D60">
-        <v>0.77800000000000002</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="E60">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2380,19 +2377,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C61">
         <v>-1</v>
       </c>
       <c r="D61">
-        <v>0.78500000000000003</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="E61">
-        <v>0.222</v>
+        <v>0.5</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2404,22 +2401,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="C62">
-        <v>65</v>
+        <v>-1</v>
       </c>
       <c r="D62">
-        <v>0.78500000000000003</v>
+        <v>0.82</v>
       </c>
       <c r="E62">
-        <v>0.25</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62">
         <f>IF(A62=B62, 1, 0)</f>
@@ -2428,19 +2425,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C63">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D63">
-        <v>0.81</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E63">
-        <v>0.25</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -2476,19 +2473,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C65">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D65">
-        <v>0.81799999999999995</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="E65">
-        <v>0.222</v>
+        <v>0.375</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -2500,22 +2497,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C66">
-        <v>-1</v>
+        <v>33</v>
       </c>
       <c r="D66">
-        <v>0.82</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="E66">
-        <v>0.33300000000000002</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <f>IF(A66=B66, 1, 0)</f>
@@ -2524,19 +2521,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C67">
         <v>-1</v>
       </c>
       <c r="D67">
-        <v>0.82499999999999996</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E67">
-        <v>0.375</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2548,22 +2545,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C68">
-        <v>-1</v>
+        <v>88</v>
       </c>
       <c r="D68">
-        <v>0.84099999999999997</v>
+        <v>0.66300000000000003</v>
       </c>
       <c r="E68">
-        <v>0.33300000000000002</v>
+        <v>0.222</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <f>IF(A68=B68, 1, 0)</f>
@@ -2572,16 +2569,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C69">
         <v>-1</v>
       </c>
       <c r="D69">
-        <v>0.84399999999999997</v>
+        <v>0.19400000000000001</v>
       </c>
       <c r="E69">
         <v>0.42899999999999999</v>
@@ -2596,19 +2593,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C70">
         <v>-1</v>
       </c>
       <c r="D70">
-        <v>0.84599999999999997</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="E70">
-        <v>0.375</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2620,19 +2617,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="C71">
         <v>-1</v>
       </c>
       <c r="D71">
-        <v>0.85299999999999998</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="E71">
-        <v>0.222</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2644,22 +2641,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C72">
-        <v>-1</v>
+        <v>23</v>
       </c>
       <c r="D72">
-        <v>0.85899999999999999</v>
+        <v>0.81</v>
       </c>
       <c r="E72">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72">
         <f>IF(A72=B72, 1, 0)</f>
@@ -2668,22 +2665,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C73">
-        <v>-1</v>
+        <v>76</v>
       </c>
       <c r="D73">
-        <v>0.86099999999999999</v>
+        <v>0.875</v>
       </c>
       <c r="E73">
-        <v>0.33300000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73">
         <f>IF(A73=B73, 1, 0)</f>
@@ -2692,19 +2689,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C74">
         <v>-1</v>
       </c>
       <c r="D74">
-        <v>0.86299999999999999</v>
+        <v>0.39700000000000002</v>
       </c>
       <c r="E74">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2716,22 +2713,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C75">
-        <v>-1</v>
+        <v>85</v>
       </c>
       <c r="D75">
-        <v>0.87</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="E75">
-        <v>0.33300000000000002</v>
+        <v>0.111</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G75">
         <f>IF(A75=B75, 1, 0)</f>
@@ -2740,22 +2737,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C76">
-        <v>-1</v>
+        <v>67</v>
       </c>
       <c r="D76">
-        <v>0.871</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="E76">
         <v>0.375</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76">
         <f>IF(A76=B76, 1, 0)</f>
@@ -2764,22 +2761,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="C77">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="D77">
-        <v>0.873</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="E77">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77">
         <f>IF(A77=B77, 1, 0)</f>
@@ -2788,22 +2785,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C78">
-        <v>76</v>
+        <v>-1</v>
       </c>
       <c r="D78">
-        <v>0.875</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="E78">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78">
         <f>IF(A78=B78, 1, 0)</f>
@@ -2812,16 +2809,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C79">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="D79">
-        <v>0.879</v>
+        <v>0.81799999999999995</v>
       </c>
       <c r="E79">
         <v>0.222</v>
@@ -2836,19 +2833,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>-1</v>
       </c>
       <c r="D80">
-        <v>0.88100000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="E80">
-        <v>0.42899999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2860,19 +2857,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="C81">
         <v>-1</v>
       </c>
       <c r="D81">
-        <v>0.88300000000000001</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="E81">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2884,22 +2881,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C82">
-        <v>88</v>
+        <v>-1</v>
       </c>
       <c r="D82">
-        <v>0.88300000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E82">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82">
         <f>IF(A82=B82, 1, 0)</f>
@@ -2908,19 +2905,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="C83">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="D83">
-        <v>0.88400000000000001</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="E83">
-        <v>0.222</v>
+        <v>0.375</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -2932,22 +2929,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="C84">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="D84">
-        <v>0.88700000000000001</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="E84">
-        <v>0.222</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
         <f>IF(A84=B84, 1, 0)</f>
@@ -2956,22 +2953,22 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="C85">
-        <v>-1</v>
+        <v>88</v>
       </c>
       <c r="D85">
-        <v>0.88700000000000001</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="E85">
-        <v>0.42899999999999999</v>
+        <v>0.375</v>
       </c>
       <c r="F85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85">
         <f>IF(A85=B85, 1, 0)</f>
@@ -2980,22 +2977,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="C86">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="D86">
-        <v>0.89100000000000001</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="E86">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86">
         <f>IF(A86=B86, 1, 0)</f>
@@ -3004,22 +3001,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C87">
-        <v>-1</v>
+        <v>73</v>
       </c>
       <c r="D87">
-        <v>0.89600000000000002</v>
+        <v>0.753</v>
       </c>
       <c r="E87">
-        <v>0.33300000000000002</v>
+        <v>0.222</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87">
         <f>IF(A87=B87, 1, 0)</f>
@@ -3028,22 +3025,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C88">
-        <v>53</v>
+        <v>-1</v>
       </c>
       <c r="D88">
-        <v>0.90100000000000002</v>
+        <v>0.871</v>
       </c>
       <c r="E88">
         <v>0.375</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88">
         <f>IF(A88=B88, 1, 0)</f>
@@ -3052,19 +3049,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C89">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="D89">
-        <v>0.90100000000000002</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="E89">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F89">
         <v>0</v>
@@ -3076,22 +3073,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C90">
-        <v>67</v>
+        <v>-1</v>
       </c>
       <c r="D90">
-        <v>0.91300000000000003</v>
+        <v>0.73</v>
       </c>
       <c r="E90">
         <v>0.375</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90">
         <f>IF(A90=B90, 1, 0)</f>
@@ -3100,22 +3097,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C91">
-        <v>93</v>
+        <v>-1</v>
       </c>
       <c r="D91">
-        <v>0.92700000000000005</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="E91">
-        <v>0.375</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91">
         <f>IF(A91=B91, 1, 0)</f>
@@ -3124,22 +3121,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="C92">
-        <v>-1</v>
+        <v>60</v>
       </c>
       <c r="D92">
-        <v>0.92900000000000005</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="E92">
-        <v>0.33300000000000002</v>
+        <v>0.222</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G92">
         <f>IF(A92=B92, 1, 0)</f>
@@ -3148,22 +3145,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="C93">
-        <v>-1</v>
+        <v>90</v>
       </c>
       <c r="D93">
-        <v>0.97099999999999997</v>
+        <v>0.24099999999999999</v>
       </c>
       <c r="E93">
-        <v>0.33300000000000002</v>
+        <v>0.111</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G93">
         <f>IF(A93=B93, 1, 0)</f>
@@ -3172,19 +3169,19 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="C94">
         <v>-1</v>
       </c>
       <c r="D94">
-        <v>0.97299999999999998</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="E94">
-        <v>0.57099999999999995</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3196,19 +3193,19 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C95">
         <v>-1</v>
       </c>
       <c r="D95">
-        <v>0.97599999999999998</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="E95">
-        <v>0.33300000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3220,22 +3217,22 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C96">
-        <v>-1</v>
+        <v>65</v>
       </c>
       <c r="D96">
-        <v>0.98099999999999998</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="E96">
-        <v>0.33300000000000002</v>
+        <v>0.25</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96">
         <f>IF(A96=B96, 1, 0)</f>
@@ -3244,19 +3241,19 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="C97">
         <v>-1</v>
       </c>
       <c r="D97">
-        <v>0.98499999999999999</v>
+        <v>0.443</v>
       </c>
       <c r="E97">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -3268,22 +3265,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="C98">
-        <v>-1</v>
+        <v>73</v>
       </c>
       <c r="D98">
-        <v>0.98599999999999999</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="E98">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98">
         <f>IF(A98=B98, 1, 0)</f>
@@ -3292,16 +3289,16 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C99">
         <v>-1</v>
       </c>
       <c r="D99">
-        <v>0.98699999999999999</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="E99">
         <v>0.5</v>
@@ -3316,22 +3313,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C100">
-        <v>-1</v>
+        <v>73</v>
       </c>
       <c r="D100">
-        <v>0.98799999999999999</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="E100">
-        <v>0.5</v>
+        <v>0.111</v>
       </c>
       <c r="F100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G100">
         <f>IF(A100=B100, 1, 0)</f>
@@ -3340,22 +3337,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="C101">
-        <v>-1</v>
+        <v>100</v>
       </c>
       <c r="D101">
-        <v>0.98899999999999999</v>
+        <v>0.753</v>
       </c>
       <c r="E101">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G101">
         <f>IF(A101=B101, 1, 0)</f>
@@ -3364,22 +3361,22 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="C102">
-        <v>-1</v>
+        <v>99</v>
       </c>
       <c r="D102">
-        <v>0.98899999999999999</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="E102">
-        <v>0.57099999999999995</v>
+        <v>0.375</v>
       </c>
       <c r="F102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G102">
         <f>IF(A102=B102, 1, 0)</f>

</xml_diff>